<commit_message>
readme updates and making better names of files
</commit_message>
<xml_diff>
--- a/PCB_files/cal-boards-panelization1-bom.xlsx
+++ b/PCB_files/cal-boards-panelization1-bom.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\lafe\MEMS switches\pcb layout\calboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DCC5F19-79C0-4013-BC5D-A3DFC02E076E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814BD9D-E47E-4CA4-A374-E3875264C47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{F1C2F2D3-E0C9-4FF4-AAD3-C74A0A44E14E}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="12735" xr2:uid="{B1787FC1-9F8F-4380-AC83-C3778B769DCD}"/>
   </bookViews>
   <sheets>
-    <sheet name="cal-boards-panelization1-bom" sheetId="1" r:id="rId1"/>
+    <sheet name="mems-switches-rectangle11" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'cal-boards-panelization1-bom'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'mems-switches-rectangle11'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -53,22 +50,64 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>LibRef</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
+    <t>Mfgr</t>
+  </si>
+  <si>
+    <t>Mfgr Part No.</t>
+  </si>
+  <si>
+    <t>rosenberger-19S201-40ML5</t>
+  </si>
+  <si>
+    <t>0201-resistor</t>
+  </si>
+  <si>
+    <t>TE connectivity</t>
+  </si>
+  <si>
+    <t>Rosenberger</t>
+  </si>
+  <si>
     <t>Fiducial</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>[NoValue], 1, 2, 3, 4, 5</t>
-  </si>
-  <si>
     <t>fiducial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>50 Ohm resistor</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6</t>
+  </si>
+  <si>
+    <t>CPF0201B49R9E1</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5,6</t>
+  </si>
+  <si>
+    <t>SMP-straight-19S10H-40ML5</t>
+  </si>
+  <si>
+    <t>SMP-straight-19S141-40ML5</t>
+  </si>
+  <si>
+    <t>J1,J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>19S141-40ML5</t>
+  </si>
+  <si>
+    <t>19S10H-40ML5</t>
   </si>
 </sst>
 </file>
@@ -444,17 +483,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4ECD5D-ECF8-41D5-8CE0-7A92766766E2}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372DEF32-082F-4A64-A2B3-410484F1FE31}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -474,24 +518,123 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>78</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1">
-        <v>6</v>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>